<commit_message>
updated relevance and apptempts when we created new code
</commit_message>
<xml_diff>
--- a/upload/payment/счет_24546799.xlsx
+++ b/upload/payment/счет_24546799.xlsx
@@ -772,7 +772,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
@@ -800,7 +800,7 @@
       </c>
       <c r="C2" s="16" t="inlineStr">
         <is>
-          <t>ООО "ДЕЛОВОЙ КЛУБ"</t>
+          <t>ООО "КМС"</t>
         </is>
       </c>
     </row>
@@ -818,7 +818,7 @@
       <c r="B4" s="10" t="n"/>
       <c r="C4" s="15" t="inlineStr">
         <is>
-          <t>ИНН 9715357887 КПП 771501001                         40702810338000156966</t>
+          <t xml:space="preserve">  ИНН 7725731508 КПП 772501001             40702810838000108799</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="22" t="inlineStr">
         <is>
-          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых". По Договору оказания услуг ФЛМ-24546799 от 5.10.21</t>
+          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546799 от 25.10.21</t>
         </is>
       </c>
     </row>
@@ -872,7 +872,7 @@
       <c r="B10" s="10" t="n"/>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>75000</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="C15" s="16" t="inlineStr">
         <is>
-          <t>ООО "ДЕЛОВОЙ КЛУБ"</t>
+          <t>ООО "КМС"</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       <c r="B17" s="10" t="n"/>
       <c r="C17" s="15" t="inlineStr">
         <is>
-          <t>ИНН 9715357887 КПП 771501001                         40702810338000156966</t>
+          <t xml:space="preserve">  ИНН 7725731508 КПП 772501001             40702810838000108799</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       <c r="B21" s="10" t="n"/>
       <c r="C21" s="11" t="inlineStr">
         <is>
-          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых". По Договору оказания услуг ФЛМ-24546799 от 5.10.21</t>
+          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546799 от 25.10.21</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       <c r="B23" s="5" t="n"/>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>75000</t>
         </is>
       </c>
     </row>

</xml_diff>